<commit_message>
feat: Add the project, display button
Display every button for each country where we have statistic
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\plot-that-lines\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E07F2BC-BE6D-4558-A9A6-4B82E1624711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4BDD8D-4467-45FB-AD7E-CCF69A2D1EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>https://etml.icescrum.com/p/PLOTTHATLI/#/taskBoard/1289</t>
+  </si>
+  <si>
+    <t>Écouter les instructions, mettre en place le travail et se rappeler du travail effectué</t>
   </si>
 </sst>
 </file>
@@ -607,7 +610,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -671,7 +674,7 @@
       </c>
       <c r="C3" s="21">
         <f>SUM(C5:C521)</f>
-        <v>0.13194444444444445</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -809,14 +812,22 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="str">
+      <c r="A11" s="14">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="B11" s="9">
+        <v>45541</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -6580,6 +6591,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6802,27 +6833,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6839,23 +6869,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(work diary): update work diary
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\plot-that-lines\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5636FF9-4BF0-46B7-B66A-A439673EE11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B18177-243B-4D2C-B7EA-DCDD022389EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -140,6 +140,21 @@
     <t>Lire un CSV et afficher un bouton pour chaque pays dans le CSV. 
 M'a pris ~1h puis les boutons étaient mal positionnés donc j'ai dû définir leurs largeur selon leurs taille
 J'ai aussi dû supprimer des jeux de donnée vide</t>
+  </si>
+  <si>
+    <t>Daily Scrum puis information sur les conventions de nommage des commits.</t>
+  </si>
+  <si>
+    <t>Créer une seconde fenêtre lorsque l'on clique sur un bouton</t>
+  </si>
+  <si>
+    <t>Afficher le graphique du pays</t>
+  </si>
+  <si>
+    <t>https://scottplot.net/cookbook/5.0/Callout/CalloutQuickstart/</t>
+  </si>
+  <si>
+    <t>J'essaye d'afficher les informations d'un point lorsque la souris passe dessus, je n'ai pas trouvé comment faire cela dans la documentation.</t>
   </si>
 </sst>
 </file>
@@ -304,6 +319,50 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -352,50 +411,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -410,7 +425,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A5:F531" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}">
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -418,14 +433,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(B6),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -620,8 +635,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="5" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -685,7 +700,7 @@
       </c>
       <c r="C3" s="21">
         <f>SUM(C5:C521)</f>
-        <v>0.25</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -833,7 +848,7 @@
       <c r="C11" s="10">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -852,7 +867,7 @@
       <c r="C12" s="10">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -873,7 +888,7 @@
       <c r="C13" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="22" t="s">
@@ -882,48 +897,82 @@
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="str">
+      <c r="A14" s="14">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45548</v>
+      </c>
+      <c r="C14" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="str">
+      <c r="A15" s="14">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45548</v>
+      </c>
+      <c r="C15" s="10">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="str">
+      <c r="A16" s="14">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45548</v>
+      </c>
+      <c r="C16" s="10">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="str">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="B17" s="9">
+        <v>45548</v>
+      </c>
+      <c r="C17" s="10">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="str">
@@ -6585,19 +6634,19 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D531">
-    <cfRule type="expression" dxfId="12" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
       <formula>$D6="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$D6="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>$D6="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>$D6="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
       <formula>$D6="Dévelopement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6610,36 +6659,17 @@
     <hyperlink ref="F6" r:id="rId1" xr:uid="{B508F36C-320A-4093-9063-F4DA4F4B5FF1}"/>
     <hyperlink ref="F8" r:id="rId2" xr:uid="{138C51BA-3627-4EA1-B9D2-CD1DD6E29056}"/>
     <hyperlink ref="F10" r:id="rId3" location="/taskBoard/1289" xr:uid="{C8F3CEBB-A200-49D3-8D35-4F56258BCD3C}"/>
+    <hyperlink ref="F17" r:id="rId4" xr:uid="{F053DE6A-CBAB-4534-8894-DA5EC5F7F779}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6862,26 +6892,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6898,4 +6929,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(work diary): Add the work diary of 27.09.2024
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\plot-that-lines\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B18177-243B-4D2C-B7EA-DCDD022389EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38B6C57-F8D8-4B46-ABB1-8261E6659D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -155,6 +155,36 @@
   </si>
   <si>
     <t>J'essaye d'afficher les informations d'un point lorsque la souris passe dessus, je n'ai pas trouvé comment faire cela dans la documentation.</t>
+  </si>
+  <si>
+    <t>Daily Scrum et écouter les informations, préparer les outils pour travailler</t>
+  </si>
+  <si>
+    <t>Je refais une maquette sur papier</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/14058412/passing-parameter-to-an-event-handler/14058441#14058441</t>
+  </si>
+  <si>
+    <t>Je change l'interface de mon application pour enlever tous les boutons et mettre une liste à la place, je n'arrivais plus à rouvrir une nouvelle fenêtre sans les boutons.</t>
+  </si>
+  <si>
+    <t>Imprévu</t>
+  </si>
+  <si>
+    <t>Connexion internet ne fonctionne plus</t>
+  </si>
+  <si>
+    <t>Je cherche une API permettant de convertir mes données (qui sont dans la devise du pays en euro)</t>
+  </si>
+  <si>
+    <t>https://currency.getgeoapi.com/documentation/#currency-convert</t>
+  </si>
+  <si>
+    <t>J'arrive à lire des éléments d'une API</t>
+  </si>
+  <si>
+    <t>J'essaie de convertir une devise en une autre depuis l'api</t>
   </si>
 </sst>
 </file>
@@ -317,7 +347,109 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -425,7 +557,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A5:F531" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}">
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -433,14 +565,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="22">
       <calculatedColumnFormula>IF(ISBLANK(B6),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -635,8 +767,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -646,12 +778,13 @@
     <col min="3" max="3" width="13.875" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.875" customWidth="1"/>
     <col min="5" max="5" width="83.5" customWidth="1"/>
-    <col min="6" max="6" width="72.125" customWidth="1"/>
-    <col min="10" max="10" width="7.5" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="13.125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13.625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="91.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5" customWidth="1"/>
+    <col min="14" max="14" width="2.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
@@ -678,6 +811,9 @@
       <c r="F2" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
       <c r="J2" t="s">
         <v>7</v>
       </c>
@@ -700,7 +836,7 @@
       </c>
       <c r="C3" s="21">
         <f>SUM(C5:C521)</f>
-        <v>0.36458333333333331</v>
+        <v>0.49652777777777773</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -975,80 +1111,140 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="str">
+      <c r="A18" s="14">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="B18" s="9">
+        <v>45562</v>
+      </c>
+      <c r="C18" s="10">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="str">
+      <c r="A19" s="14">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="B19" s="9">
+        <v>45562</v>
+      </c>
+      <c r="C19" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="str">
+    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="B20" s="9">
+        <v>45562</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="str">
+      <c r="A21" s="14">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="B21" s="9">
+        <v>45562</v>
+      </c>
+      <c r="C21" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="str">
+      <c r="A22" s="14">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="B22" s="9">
+        <v>45562</v>
+      </c>
+      <c r="C22" s="10">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="str">
+      <c r="A23" s="14">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="B23" s="9">
+        <v>45562</v>
+      </c>
+      <c r="C23" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="str">
+      <c r="A24" s="14">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="B24" s="9">
+        <v>45562</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -6634,42 +6830,70 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D531">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="2" stopIfTrue="1">
       <formula>$D6="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>$D6="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>$D6="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="5" stopIfTrue="1">
       <formula>$D6="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>$D6="Dévelopement"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D531" xr:uid="{286A9366-4079-8F4A-9AB6-501A4911E2F7}">
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>$D$21="Imprévu"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D20 D22:D531" xr:uid="{286A9366-4079-8F4A-9AB6-501A4911E2F7}">
       <formula1>$I$2:$N$2</formula1>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D21" xr:uid="{D1921438-8888-4759-B714-95B9313172E3}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{B508F36C-320A-4093-9063-F4DA4F4B5FF1}"/>
     <hyperlink ref="F8" r:id="rId2" xr:uid="{138C51BA-3627-4EA1-B9D2-CD1DD6E29056}"/>
     <hyperlink ref="F10" r:id="rId3" location="/taskBoard/1289" xr:uid="{C8F3CEBB-A200-49D3-8D35-4F56258BCD3C}"/>
     <hyperlink ref="F17" r:id="rId4" xr:uid="{F053DE6A-CBAB-4534-8894-DA5EC5F7F779}"/>
+    <hyperlink ref="F20" r:id="rId5" location="14058441" xr:uid="{43179A56-F5C8-4E66-9711-A6B301391286}"/>
+    <hyperlink ref="F22" r:id="rId6" location="currency-convert" xr:uid="{6737EA30-0222-4AE0-A6B6-524639736439}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6892,27 +7116,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6929,23 +7152,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(work diary): update the work diary of 11.10.2024
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\plot-that-lines\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C54BDC8-D794-4E51-B021-0CDBD88FDAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEA9CD0-10C9-4AD7-A344-1E7C5ED9D473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -207,6 +207,24 @@
   <si>
     <t>Clean le code, utiliser des fonctions</t>
   </si>
+  <si>
+    <t>Écouter les instructions du professeur. Daily Scrum.</t>
+  </si>
+  <si>
+    <t>Pause pour aller discuter avec mon professeur principal</t>
+  </si>
+  <si>
+    <t>Je reviens lors d'une explication sur PlantUML et IceTools</t>
+  </si>
+  <si>
+    <t>Je recrée une nouvelle maquette papier après discussion avec le professeur car mon application servirait plus à comparer les dépenses militaires entre pays ce qui n'est pas assez montré sur la maquette actuelle.</t>
+  </si>
+  <si>
+    <t>Je crée mes exceptions de filtrage. J'ai des problèmes car je n'utilise pas les valeurs modifiés.</t>
+  </si>
+  <si>
+    <t>Je refactorise mon code</t>
+  </si>
 </sst>
 </file>
 
@@ -268,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -361,6 +385,9 @@
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -693,8 +720,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -762,7 +789,7 @@
       </c>
       <c r="C3" s="21">
         <f>SUM(C5:C521)</f>
-        <v>0.6875</v>
+        <v>0.82638888888888873</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1294,69 +1321,117 @@
       <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="str">
+      <c r="A31" s="14">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="B31" s="9">
+        <v>45576</v>
+      </c>
+      <c r="C31" s="10">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="str">
+      <c r="A32" s="14">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="B32" s="9">
+        <v>45576</v>
+      </c>
+      <c r="C32" s="10">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="str">
+      <c r="A33" s="14">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="B33" s="9">
+        <v>45576</v>
+      </c>
+      <c r="C33" s="10">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="str">
+    <row r="34" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="B34" s="9">
+        <v>45576</v>
+      </c>
+      <c r="C34" s="10">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="str">
+      <c r="A35" s="14">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="B35" s="9">
+        <v>45576</v>
+      </c>
+      <c r="C35" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="str">
+      <c r="A36" s="14">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="B36" s="9">
+        <v>45576</v>
+      </c>
+      <c r="C36" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -6855,12 +6930,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7087,20 +7164,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7125,12 +7203,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(work diary): update the work diary of the 24.10.2024
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyco\Documents\GitHub\plot-that-lines\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27D8D2E-DD24-480B-9444-163EAECEF457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAFB972-B895-4223-93A6-DE9E84B22670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -236,6 +236,18 @@
   </si>
   <si>
     <t>J'essaie de convertir une devise en une autre depuis l'api. Pas encore réussi.</t>
+  </si>
+  <si>
+    <t>J'avance dans le rapport à fournir.</t>
+  </si>
+  <si>
+    <t>J'essaie de créer un projet de test, j'avais des erreurs de compatibilité.</t>
+  </si>
+  <si>
+    <t>Je crée les tests unitaires, je m'aide de ChatGPT pour qu'il m'aide à identifier tous les points à tester (je n'avais pas pensé à tester des valeurs incorrect, etc)</t>
+  </si>
+  <si>
+    <t>J'analyse mon code, je corrige une erreur et je réfléchi à comment le rendre plus simple et plus lisible</t>
   </si>
 </sst>
 </file>
@@ -731,9 +743,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -801,7 +813,7 @@
       </c>
       <c r="C3" s="21">
         <f>SUM(C5:C521)</f>
-        <v>0.97916666666666641</v>
+        <v>1.1111111111111107</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1523,58 +1535,98 @@
       <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="14" t="str">
+      <c r="A41" s="14">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B41" s="9">
+        <v>45589</v>
+      </c>
+      <c r="C41" s="10">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="14" t="str">
+      <c r="A42" s="14">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B42" s="9">
+        <v>45589</v>
+      </c>
+      <c r="C42" s="10">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="F42" s="11"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="14" t="str">
+    <row r="43" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="A43" s="14">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B43" s="9">
+        <v>45589</v>
+      </c>
+      <c r="C43" s="10">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>67</v>
+      </c>
       <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="14" t="str">
+      <c r="A44" s="14">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="9">
+        <v>45589</v>
+      </c>
+      <c r="C44" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="14" t="str">
+      <c r="A45" s="14">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B45" s="9">
+        <v>45589</v>
+      </c>
+      <c r="C45" s="10">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
docs(work diary): display the total time in hours
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyco\Documents\GitHub\plot-that-lines\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAFB972-B895-4223-93A6-DE9E84B22670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C0EC7D-BDF3-43F9-BCED-4F52B48B94FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Auteur:</t>
-  </si>
-  <si>
-    <t>Berchel joachim</t>
   </si>
   <si>
     <t>P_FUN</t>
@@ -249,13 +246,17 @@
   <si>
     <t>J'analyse mon code, je corrige une erreur et je réfléchi à comment le rendre plus simple et plus lisible</t>
   </si>
+  <si>
+    <t>Berchel Joachim</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$]dd/mm/yyyy;@" x16r2:formatCode16="[$-en-CH,1]dd/mm/yyyy;@"/>
+    <numFmt numFmtId="168" formatCode="[hh]:mm:ss"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -388,7 +389,6 @@
     <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
@@ -398,9 +398,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
@@ -414,6 +411,10 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -744,8 +745,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -778,18 +779,18 @@
       <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="28"/>
+      <c r="C2" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="26"/>
       <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
         <v>7</v>
@@ -811,8 +812,8 @@
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="21">
-        <f>SUM(C5:C521)</f>
+      <c r="C3" s="28">
+        <f>SUM(C6:C521)</f>
         <v>1.1111111111111107</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -853,17 +854,17 @@
       <c r="B6" s="9">
         <v>45534</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="27">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="24" t="s">
+      <c r="E6" s="21" t="s">
         <v>19</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -874,17 +875,17 @@
       <c r="B7" s="9">
         <v>45534</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="27">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="31" x14ac:dyDescent="0.35">
@@ -895,17 +896,17 @@
       <c r="B8" s="9">
         <v>45534</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="27">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="24" t="s">
         <v>23</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -916,17 +917,17 @@
       <c r="B9" s="9">
         <v>45534</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="27">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -937,17 +938,17 @@
       <c r="B10" s="9">
         <v>45534</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="27">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -958,14 +959,14 @@
       <c r="B11" s="9">
         <v>45541</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="27">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="11"/>
     </row>
@@ -977,17 +978,17 @@
       <c r="B12" s="9">
         <v>45541</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="27">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="62" x14ac:dyDescent="0.35">
@@ -998,14 +999,14 @@
       <c r="B13" s="9">
         <v>45541</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="27">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>32</v>
+      <c r="E13" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="F13" s="11"/>
     </row>
@@ -1017,14 +1018,14 @@
       <c r="B14" s="9">
         <v>45548</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="27">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="11"/>
     </row>
@@ -1036,14 +1037,14 @@
       <c r="B15" s="9">
         <v>45548</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="27">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="11"/>
     </row>
@@ -1055,14 +1056,14 @@
       <c r="B16" s="9">
         <v>45548</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="27">
         <v>3.125E-2</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="11"/>
     </row>
@@ -1074,17 +1075,17 @@
       <c r="B17" s="9">
         <v>45548</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="27">
         <v>2.4305555555555556E-2</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="24" t="s">
+      <c r="E17" s="21" t="s">
         <v>36</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1095,14 +1096,14 @@
       <c r="B18" s="9">
         <v>45562</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="27">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="11"/>
     </row>
@@ -1114,14 +1115,14 @@
       <c r="B19" s="9">
         <v>45562</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="27">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F19" s="11"/>
     </row>
@@ -1133,17 +1134,17 @@
       <c r="B20" s="9">
         <v>45562</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="27">
         <v>3.4722222222222224E-2</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="24" t="s">
+      <c r="E20" s="21" t="s">
         <v>40</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1154,14 +1155,14 @@
       <c r="B21" s="9">
         <v>45562</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="27">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D21" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F21" s="11"/>
     </row>
@@ -1173,17 +1174,17 @@
       <c r="B22" s="9">
         <v>45562</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="27">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="23" t="s">
         <v>44</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1194,14 +1195,14 @@
       <c r="B23" s="9">
         <v>45562</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="27">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="11"/>
     </row>
@@ -1213,14 +1214,14 @@
       <c r="B24" s="9">
         <v>45562</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="27">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" s="11"/>
     </row>
@@ -1232,17 +1233,17 @@
       <c r="B25" s="9">
         <v>45563</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="27">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1253,17 +1254,17 @@
       <c r="B26" s="9">
         <v>45563</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="27">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="31" x14ac:dyDescent="0.35">
@@ -1274,14 +1275,14 @@
       <c r="B27" s="9">
         <v>45569</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="27">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="22" t="s">
-        <v>51</v>
+      <c r="E27" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="F27" s="11"/>
     </row>
@@ -1293,17 +1294,17 @@
       <c r="B28" s="9">
         <v>45569</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="27">
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>28</v>
+      <c r="E28" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
@@ -1314,14 +1315,14 @@
       <c r="B29" s="9">
         <v>45569</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="27">
         <v>9.7222222222222224E-2</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="22" t="s">
-        <v>53</v>
+      <c r="E29" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="F29" s="11"/>
     </row>
@@ -1333,14 +1334,14 @@
       <c r="B30" s="9">
         <v>45569</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="27">
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" s="11"/>
     </row>
@@ -1352,14 +1353,14 @@
       <c r="B31" s="9">
         <v>45576</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="27">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F31" s="11"/>
     </row>
@@ -1371,14 +1372,14 @@
       <c r="B32" s="9">
         <v>45576</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="27">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="D32" s="27" t="s">
-        <v>42</v>
+      <c r="D32" s="25" t="s">
+        <v>41</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1390,14 +1391,14 @@
       <c r="B33" s="9">
         <v>45576</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="27">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F33" s="11"/>
     </row>
@@ -1409,14 +1410,14 @@
       <c r="B34" s="9">
         <v>45576</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="27">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="22" t="s">
-        <v>58</v>
+      <c r="E34" s="21" t="s">
+        <v>57</v>
       </c>
       <c r="F34" s="11"/>
     </row>
@@ -1428,14 +1429,14 @@
       <c r="B35" s="9">
         <v>45576</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="27">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F35" s="11"/>
     </row>
@@ -1447,14 +1448,14 @@
       <c r="B36" s="9">
         <v>45576</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="27">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F36" s="11"/>
     </row>
@@ -1466,14 +1467,14 @@
       <c r="B37" s="9">
         <v>45588</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="27">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="22" t="s">
-        <v>61</v>
+      <c r="E37" s="21" t="s">
+        <v>60</v>
       </c>
       <c r="F37" s="11"/>
     </row>
@@ -1485,14 +1486,14 @@
       <c r="B38" s="9">
         <v>45588</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="27">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F38" s="11"/>
     </row>
@@ -1504,14 +1505,14 @@
       <c r="B39" s="9">
         <v>45588</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="27">
         <v>6.9444444444444448E-2</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F39" s="11"/>
     </row>
@@ -1523,14 +1524,14 @@
       <c r="B40" s="9">
         <v>45588</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="27">
         <v>6.25E-2</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F40" s="11"/>
     </row>
@@ -1542,14 +1543,14 @@
       <c r="B41" s="9">
         <v>45589</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="27">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41" s="11"/>
     </row>
@@ -1561,14 +1562,14 @@
       <c r="B42" s="9">
         <v>45589</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="27">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F42" s="11"/>
     </row>
@@ -1580,14 +1581,14 @@
       <c r="B43" s="9">
         <v>45589</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="27">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="22" t="s">
-        <v>67</v>
+      <c r="E43" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="F43" s="11"/>
     </row>
@@ -1599,14 +1600,14 @@
       <c r="B44" s="9">
         <v>45589</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="27">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F44" s="11"/>
     </row>
@@ -1618,14 +1619,14 @@
       <c r="B45" s="9">
         <v>45589</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="27">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F45" s="11"/>
     </row>
@@ -1635,7 +1636,7 @@
         <v/>
       </c>
       <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
@@ -1646,7 +1647,7 @@
         <v/>
       </c>
       <c r="B47" s="9"/>
-      <c r="C47" s="10"/>
+      <c r="C47" s="27"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
@@ -1657,7 +1658,7 @@
         <v/>
       </c>
       <c r="B48" s="9"/>
-      <c r="C48" s="10"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
@@ -1668,7 +1669,7 @@
         <v/>
       </c>
       <c r="B49" s="9"/>
-      <c r="C49" s="10"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
@@ -1679,7 +1680,7 @@
         <v/>
       </c>
       <c r="B50" s="9"/>
-      <c r="C50" s="10"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
@@ -1690,7 +1691,7 @@
         <v/>
       </c>
       <c r="B51" s="9"/>
-      <c r="C51" s="10"/>
+      <c r="C51" s="27"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -1701,7 +1702,7 @@
         <v/>
       </c>
       <c r="B52" s="9"/>
-      <c r="C52" s="10"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
@@ -1712,7 +1713,7 @@
         <v/>
       </c>
       <c r="B53" s="9"/>
-      <c r="C53" s="10"/>
+      <c r="C53" s="27"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
@@ -1723,7 +1724,7 @@
         <v/>
       </c>
       <c r="B54" s="9"/>
-      <c r="C54" s="10"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
@@ -1734,7 +1735,7 @@
         <v/>
       </c>
       <c r="B55" s="9"/>
-      <c r="C55" s="10"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -1745,7 +1746,7 @@
         <v/>
       </c>
       <c r="B56" s="9"/>
-      <c r="C56" s="10"/>
+      <c r="C56" s="27"/>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
@@ -1756,7 +1757,7 @@
         <v/>
       </c>
       <c r="B57" s="9"/>
-      <c r="C57" s="10"/>
+      <c r="C57" s="27"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
@@ -1767,7 +1768,7 @@
         <v/>
       </c>
       <c r="B58" s="9"/>
-      <c r="C58" s="10"/>
+      <c r="C58" s="27"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
@@ -1778,7 +1779,7 @@
         <v/>
       </c>
       <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
+      <c r="C59" s="27"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
@@ -1789,7 +1790,7 @@
         <v/>
       </c>
       <c r="B60" s="9"/>
-      <c r="C60" s="10"/>
+      <c r="C60" s="27"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -1800,7 +1801,7 @@
         <v/>
       </c>
       <c r="B61" s="9"/>
-      <c r="C61" s="10"/>
+      <c r="C61" s="27"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
@@ -1811,7 +1812,7 @@
         <v/>
       </c>
       <c r="B62" s="9"/>
-      <c r="C62" s="10"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -1822,7 +1823,7 @@
         <v/>
       </c>
       <c r="B63" s="9"/>
-      <c r="C63" s="10"/>
+      <c r="C63" s="27"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
@@ -1833,7 +1834,7 @@
         <v/>
       </c>
       <c r="B64" s="9"/>
-      <c r="C64" s="10"/>
+      <c r="C64" s="27"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
@@ -1844,7 +1845,7 @@
         <v/>
       </c>
       <c r="B65" s="9"/>
-      <c r="C65" s="10"/>
+      <c r="C65" s="27"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
@@ -1855,7 +1856,7 @@
         <v/>
       </c>
       <c r="B66" s="9"/>
-      <c r="C66" s="10"/>
+      <c r="C66" s="27"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
@@ -1866,7 +1867,7 @@
         <v/>
       </c>
       <c r="B67" s="9"/>
-      <c r="C67" s="10"/>
+      <c r="C67" s="27"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
@@ -1877,7 +1878,7 @@
         <v/>
       </c>
       <c r="B68" s="9"/>
-      <c r="C68" s="10"/>
+      <c r="C68" s="27"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
@@ -1888,7 +1889,7 @@
         <v/>
       </c>
       <c r="B69" s="9"/>
-      <c r="C69" s="10"/>
+      <c r="C69" s="27"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
@@ -1899,7 +1900,7 @@
         <v/>
       </c>
       <c r="B70" s="9"/>
-      <c r="C70" s="10"/>
+      <c r="C70" s="27"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -1910,7 +1911,7 @@
         <v/>
       </c>
       <c r="B71" s="9"/>
-      <c r="C71" s="10"/>
+      <c r="C71" s="27"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
@@ -1921,7 +1922,7 @@
         <v/>
       </c>
       <c r="B72" s="9"/>
-      <c r="C72" s="10"/>
+      <c r="C72" s="27"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
@@ -1932,7 +1933,7 @@
         <v/>
       </c>
       <c r="B73" s="9"/>
-      <c r="C73" s="10"/>
+      <c r="C73" s="27"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
@@ -1943,7 +1944,7 @@
         <v/>
       </c>
       <c r="B74" s="9"/>
-      <c r="C74" s="10"/>
+      <c r="C74" s="27"/>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
@@ -1954,7 +1955,7 @@
         <v/>
       </c>
       <c r="B75" s="9"/>
-      <c r="C75" s="10"/>
+      <c r="C75" s="27"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
       <c r="F75" s="11"/>
@@ -1965,7 +1966,7 @@
         <v/>
       </c>
       <c r="B76" s="9"/>
-      <c r="C76" s="10"/>
+      <c r="C76" s="27"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
@@ -1976,7 +1977,7 @@
         <v/>
       </c>
       <c r="B77" s="9"/>
-      <c r="C77" s="10"/>
+      <c r="C77" s="27"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
@@ -1987,7 +1988,7 @@
         <v/>
       </c>
       <c r="B78" s="9"/>
-      <c r="C78" s="10"/>
+      <c r="C78" s="27"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
@@ -1998,7 +1999,7 @@
         <v/>
       </c>
       <c r="B79" s="9"/>
-      <c r="C79" s="10"/>
+      <c r="C79" s="27"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
@@ -2009,7 +2010,7 @@
         <v/>
       </c>
       <c r="B80" s="9"/>
-      <c r="C80" s="10"/>
+      <c r="C80" s="27"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
       <c r="F80" s="11"/>
@@ -2020,7 +2021,7 @@
         <v/>
       </c>
       <c r="B81" s="9"/>
-      <c r="C81" s="10"/>
+      <c r="C81" s="27"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
@@ -2031,7 +2032,7 @@
         <v/>
       </c>
       <c r="B82" s="9"/>
-      <c r="C82" s="10"/>
+      <c r="C82" s="27"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
       <c r="F82" s="11"/>
@@ -2042,7 +2043,7 @@
         <v/>
       </c>
       <c r="B83" s="9"/>
-      <c r="C83" s="10"/>
+      <c r="C83" s="27"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
@@ -2053,7 +2054,7 @@
         <v/>
       </c>
       <c r="B84" s="9"/>
-      <c r="C84" s="10"/>
+      <c r="C84" s="27"/>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
       <c r="F84" s="11"/>
@@ -2064,7 +2065,7 @@
         <v/>
       </c>
       <c r="B85" s="9"/>
-      <c r="C85" s="10"/>
+      <c r="C85" s="27"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
       <c r="F85" s="11"/>
@@ -2075,7 +2076,7 @@
         <v/>
       </c>
       <c r="B86" s="9"/>
-      <c r="C86" s="10"/>
+      <c r="C86" s="27"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
@@ -2086,7 +2087,7 @@
         <v/>
       </c>
       <c r="B87" s="9"/>
-      <c r="C87" s="10"/>
+      <c r="C87" s="27"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
@@ -2097,7 +2098,7 @@
         <v/>
       </c>
       <c r="B88" s="9"/>
-      <c r="C88" s="10"/>
+      <c r="C88" s="27"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
@@ -2108,7 +2109,7 @@
         <v/>
       </c>
       <c r="B89" s="9"/>
-      <c r="C89" s="10"/>
+      <c r="C89" s="27"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
@@ -2119,7 +2120,7 @@
         <v/>
       </c>
       <c r="B90" s="9"/>
-      <c r="C90" s="10"/>
+      <c r="C90" s="27"/>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
@@ -2130,7 +2131,7 @@
         <v/>
       </c>
       <c r="B91" s="9"/>
-      <c r="C91" s="10"/>
+      <c r="C91" s="27"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
@@ -2141,7 +2142,7 @@
         <v/>
       </c>
       <c r="B92" s="9"/>
-      <c r="C92" s="10"/>
+      <c r="C92" s="27"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
       <c r="F92" s="11"/>
@@ -2152,7 +2153,7 @@
         <v/>
       </c>
       <c r="B93" s="9"/>
-      <c r="C93" s="10"/>
+      <c r="C93" s="27"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
       <c r="F93" s="11"/>
@@ -2163,7 +2164,7 @@
         <v/>
       </c>
       <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
+      <c r="C94" s="27"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
       <c r="F94" s="11"/>
@@ -2174,7 +2175,7 @@
         <v/>
       </c>
       <c r="B95" s="9"/>
-      <c r="C95" s="10"/>
+      <c r="C95" s="27"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
@@ -2185,7 +2186,7 @@
         <v/>
       </c>
       <c r="B96" s="9"/>
-      <c r="C96" s="10"/>
+      <c r="C96" s="27"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
@@ -2196,7 +2197,7 @@
         <v/>
       </c>
       <c r="B97" s="9"/>
-      <c r="C97" s="10"/>
+      <c r="C97" s="27"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
@@ -2207,7 +2208,7 @@
         <v/>
       </c>
       <c r="B98" s="9"/>
-      <c r="C98" s="10"/>
+      <c r="C98" s="27"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
@@ -2218,7 +2219,7 @@
         <v/>
       </c>
       <c r="B99" s="9"/>
-      <c r="C99" s="10"/>
+      <c r="C99" s="27"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
@@ -2229,7 +2230,7 @@
         <v/>
       </c>
       <c r="B100" s="9"/>
-      <c r="C100" s="10"/>
+      <c r="C100" s="27"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
@@ -2240,7 +2241,7 @@
         <v/>
       </c>
       <c r="B101" s="9"/>
-      <c r="C101" s="10"/>
+      <c r="C101" s="27"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
       <c r="F101" s="11"/>
@@ -2251,7 +2252,7 @@
         <v/>
       </c>
       <c r="B102" s="9"/>
-      <c r="C102" s="10"/>
+      <c r="C102" s="27"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
@@ -2262,7 +2263,7 @@
         <v/>
       </c>
       <c r="B103" s="9"/>
-      <c r="C103" s="10"/>
+      <c r="C103" s="27"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
       <c r="F103" s="11"/>
@@ -2273,7 +2274,7 @@
         <v/>
       </c>
       <c r="B104" s="9"/>
-      <c r="C104" s="10"/>
+      <c r="C104" s="27"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
@@ -2284,7 +2285,7 @@
         <v/>
       </c>
       <c r="B105" s="9"/>
-      <c r="C105" s="10"/>
+      <c r="C105" s="27"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
       <c r="F105" s="11"/>
@@ -2295,7 +2296,7 @@
         <v/>
       </c>
       <c r="B106" s="9"/>
-      <c r="C106" s="10"/>
+      <c r="C106" s="27"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
       <c r="F106" s="11"/>
@@ -2306,7 +2307,7 @@
         <v/>
       </c>
       <c r="B107" s="9"/>
-      <c r="C107" s="10"/>
+      <c r="C107" s="27"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
       <c r="F107" s="11"/>
@@ -2317,7 +2318,7 @@
         <v/>
       </c>
       <c r="B108" s="9"/>
-      <c r="C108" s="10"/>
+      <c r="C108" s="27"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
@@ -2328,7 +2329,7 @@
         <v/>
       </c>
       <c r="B109" s="9"/>
-      <c r="C109" s="10"/>
+      <c r="C109" s="27"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
       <c r="F109" s="11"/>
@@ -2339,7 +2340,7 @@
         <v/>
       </c>
       <c r="B110" s="9"/>
-      <c r="C110" s="10"/>
+      <c r="C110" s="27"/>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
       <c r="F110" s="11"/>
@@ -2350,7 +2351,7 @@
         <v/>
       </c>
       <c r="B111" s="9"/>
-      <c r="C111" s="10"/>
+      <c r="C111" s="27"/>
       <c r="D111" s="11"/>
       <c r="E111" s="11"/>
       <c r="F111" s="11"/>
@@ -2361,7 +2362,7 @@
         <v/>
       </c>
       <c r="B112" s="9"/>
-      <c r="C112" s="10"/>
+      <c r="C112" s="27"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
       <c r="F112" s="11"/>
@@ -2372,7 +2373,7 @@
         <v/>
       </c>
       <c r="B113" s="9"/>
-      <c r="C113" s="10"/>
+      <c r="C113" s="27"/>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
       <c r="F113" s="11"/>
@@ -2383,7 +2384,7 @@
         <v/>
       </c>
       <c r="B114" s="9"/>
-      <c r="C114" s="10"/>
+      <c r="C114" s="27"/>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
       <c r="F114" s="11"/>
@@ -2394,7 +2395,7 @@
         <v/>
       </c>
       <c r="B115" s="9"/>
-      <c r="C115" s="10"/>
+      <c r="C115" s="27"/>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
       <c r="F115" s="11"/>
@@ -2405,7 +2406,7 @@
         <v/>
       </c>
       <c r="B116" s="9"/>
-      <c r="C116" s="10"/>
+      <c r="C116" s="27"/>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
@@ -2416,7 +2417,7 @@
         <v/>
       </c>
       <c r="B117" s="9"/>
-      <c r="C117" s="10"/>
+      <c r="C117" s="27"/>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
       <c r="F117" s="11"/>
@@ -2427,7 +2428,7 @@
         <v/>
       </c>
       <c r="B118" s="9"/>
-      <c r="C118" s="10"/>
+      <c r="C118" s="27"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
@@ -2438,7 +2439,7 @@
         <v/>
       </c>
       <c r="B119" s="9"/>
-      <c r="C119" s="10"/>
+      <c r="C119" s="27"/>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
       <c r="F119" s="11"/>
@@ -2449,7 +2450,7 @@
         <v/>
       </c>
       <c r="B120" s="9"/>
-      <c r="C120" s="10"/>
+      <c r="C120" s="27"/>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
       <c r="F120" s="11"/>
@@ -2460,7 +2461,7 @@
         <v/>
       </c>
       <c r="B121" s="9"/>
-      <c r="C121" s="10"/>
+      <c r="C121" s="27"/>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
       <c r="F121" s="11"/>
@@ -2471,7 +2472,7 @@
         <v/>
       </c>
       <c r="B122" s="9"/>
-      <c r="C122" s="10"/>
+      <c r="C122" s="27"/>
       <c r="D122" s="11"/>
       <c r="E122" s="11"/>
       <c r="F122" s="11"/>
@@ -2482,7 +2483,7 @@
         <v/>
       </c>
       <c r="B123" s="9"/>
-      <c r="C123" s="10"/>
+      <c r="C123" s="27"/>
       <c r="D123" s="11"/>
       <c r="E123" s="11"/>
       <c r="F123" s="11"/>
@@ -2493,7 +2494,7 @@
         <v/>
       </c>
       <c r="B124" s="9"/>
-      <c r="C124" s="10"/>
+      <c r="C124" s="27"/>
       <c r="D124" s="11"/>
       <c r="E124" s="11"/>
       <c r="F124" s="11"/>
@@ -2504,7 +2505,7 @@
         <v/>
       </c>
       <c r="B125" s="9"/>
-      <c r="C125" s="10"/>
+      <c r="C125" s="27"/>
       <c r="D125" s="11"/>
       <c r="E125" s="11"/>
       <c r="F125" s="11"/>
@@ -2515,7 +2516,7 @@
         <v/>
       </c>
       <c r="B126" s="9"/>
-      <c r="C126" s="10"/>
+      <c r="C126" s="27"/>
       <c r="D126" s="11"/>
       <c r="E126" s="11"/>
       <c r="F126" s="11"/>
@@ -2526,7 +2527,7 @@
         <v/>
       </c>
       <c r="B127" s="9"/>
-      <c r="C127" s="10"/>
+      <c r="C127" s="27"/>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
       <c r="F127" s="11"/>
@@ -2537,7 +2538,7 @@
         <v/>
       </c>
       <c r="B128" s="9"/>
-      <c r="C128" s="10"/>
+      <c r="C128" s="27"/>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
       <c r="F128" s="11"/>
@@ -2548,7 +2549,7 @@
         <v/>
       </c>
       <c r="B129" s="9"/>
-      <c r="C129" s="10"/>
+      <c r="C129" s="27"/>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
       <c r="F129" s="11"/>
@@ -2559,7 +2560,7 @@
         <v/>
       </c>
       <c r="B130" s="9"/>
-      <c r="C130" s="10"/>
+      <c r="C130" s="27"/>
       <c r="D130" s="11"/>
       <c r="E130" s="11"/>
       <c r="F130" s="11"/>
@@ -2570,7 +2571,7 @@
         <v/>
       </c>
       <c r="B131" s="9"/>
-      <c r="C131" s="10"/>
+      <c r="C131" s="27"/>
       <c r="D131" s="11"/>
       <c r="E131" s="11"/>
       <c r="F131" s="11"/>
@@ -2581,7 +2582,7 @@
         <v/>
       </c>
       <c r="B132" s="9"/>
-      <c r="C132" s="10"/>
+      <c r="C132" s="27"/>
       <c r="D132" s="11"/>
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
@@ -2592,7 +2593,7 @@
         <v/>
       </c>
       <c r="B133" s="9"/>
-      <c r="C133" s="10"/>
+      <c r="C133" s="27"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11"/>
       <c r="F133" s="11"/>
@@ -2603,7 +2604,7 @@
         <v/>
       </c>
       <c r="B134" s="9"/>
-      <c r="C134" s="10"/>
+      <c r="C134" s="27"/>
       <c r="D134" s="11"/>
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
@@ -2614,7 +2615,7 @@
         <v/>
       </c>
       <c r="B135" s="9"/>
-      <c r="C135" s="10"/>
+      <c r="C135" s="27"/>
       <c r="D135" s="11"/>
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
@@ -2625,7 +2626,7 @@
         <v/>
       </c>
       <c r="B136" s="9"/>
-      <c r="C136" s="10"/>
+      <c r="C136" s="27"/>
       <c r="D136" s="11"/>
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
@@ -2636,7 +2637,7 @@
         <v/>
       </c>
       <c r="B137" s="9"/>
-      <c r="C137" s="10"/>
+      <c r="C137" s="27"/>
       <c r="D137" s="11"/>
       <c r="E137" s="11"/>
       <c r="F137" s="11"/>
@@ -2647,7 +2648,7 @@
         <v/>
       </c>
       <c r="B138" s="9"/>
-      <c r="C138" s="10"/>
+      <c r="C138" s="27"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
       <c r="F138" s="11"/>
@@ -2658,7 +2659,7 @@
         <v/>
       </c>
       <c r="B139" s="9"/>
-      <c r="C139" s="10"/>
+      <c r="C139" s="27"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
       <c r="F139" s="11"/>
@@ -2669,7 +2670,7 @@
         <v/>
       </c>
       <c r="B140" s="9"/>
-      <c r="C140" s="10"/>
+      <c r="C140" s="27"/>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
       <c r="F140" s="11"/>
@@ -2680,7 +2681,7 @@
         <v/>
       </c>
       <c r="B141" s="9"/>
-      <c r="C141" s="10"/>
+      <c r="C141" s="27"/>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
       <c r="F141" s="11"/>
@@ -2691,7 +2692,7 @@
         <v/>
       </c>
       <c r="B142" s="9"/>
-      <c r="C142" s="10"/>
+      <c r="C142" s="27"/>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
       <c r="F142" s="11"/>
@@ -2702,7 +2703,7 @@
         <v/>
       </c>
       <c r="B143" s="9"/>
-      <c r="C143" s="10"/>
+      <c r="C143" s="27"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
       <c r="F143" s="11"/>
@@ -2713,7 +2714,7 @@
         <v/>
       </c>
       <c r="B144" s="9"/>
-      <c r="C144" s="10"/>
+      <c r="C144" s="27"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
       <c r="F144" s="11"/>
@@ -2724,7 +2725,7 @@
         <v/>
       </c>
       <c r="B145" s="9"/>
-      <c r="C145" s="10"/>
+      <c r="C145" s="27"/>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
       <c r="F145" s="11"/>
@@ -2735,7 +2736,7 @@
         <v/>
       </c>
       <c r="B146" s="9"/>
-      <c r="C146" s="10"/>
+      <c r="C146" s="27"/>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
       <c r="F146" s="11"/>

</xml_diff>

<commit_message>
docs(work diary): update the work diary of the 26.10.2024
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyco\Documents\GitHub\plot-that-lines\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C0EC7D-BDF3-43F9-BCED-4F52B48B94FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5208CC5-861B-40E4-9EBA-27BB43C301DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -199,9 +199,6 @@
     <t>De par les informations données par le professeur j'ai modifié mon rapport et mon IceScrum. Je n'avais pas fait attention au fait que le filtre par date soit obligatoire et j'ai donc dû le rajouter dans mes user story et mes test d'acceptance</t>
   </si>
   <si>
-    <t>J'ai eu des difficultés a accéder à certaines variables. J'ai essayé d'utiliser des fonctions de ScottPlot, au final j'ai demandé à Tiago comment il avait fait et j'ai décidé de vider mes points puis de les réafficher</t>
-  </si>
-  <si>
     <t>Clean le code, utiliser des fonctions</t>
   </si>
   <si>
@@ -249,6 +246,18 @@
   <si>
     <t>Berchel Joachim</t>
   </si>
+  <si>
+    <t>J'utilise l'API pour convertir mes données.</t>
+  </si>
+  <si>
+    <t>Il y a une limite de requête quotidienne à l'API et pour afficher un graphique il y a entre 1 et 64 requête à effectuer.</t>
+  </si>
+  <si>
+    <t>J'ai eu des difficultés a accéder à certaines variables pour la fonction de tri. J'ai essayé d'utiliser des fonctions de ScottPlot, au final j'ai demandé à Tiago comment il avait fait et j'ai décidé de vider mes points puis de les réafficher.</t>
+  </si>
+  <si>
+    <t>J'avance dans le rapport à fournir. Il ne reste plue que le IceScrub.</t>
+  </si>
 </sst>
 </file>
 
@@ -256,7 +265,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$]dd/mm/yyyy;@" x16r2:formatCode16="[$-en-CH,1]dd/mm/yyyy;@"/>
-    <numFmt numFmtId="168" formatCode="[hh]:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="[hh]:mm:ss"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -407,14 +416,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -744,9 +753,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N531"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -779,10 +788,10 @@
       <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="26"/>
+      <c r="C2" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="28"/>
       <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
@@ -812,9 +821,9 @@
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="27">
         <f>SUM(C6:C521)</f>
-        <v>1.1111111111111107</v>
+        <v>1.2152777777777775</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -854,7 +863,7 @@
       <c r="B6" s="9">
         <v>45534</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D6" s="22" t="s">
@@ -875,7 +884,7 @@
       <c r="B7" s="9">
         <v>45534</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -896,7 +905,7 @@
       <c r="B8" s="9">
         <v>45534</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D8" s="11" t="s">
@@ -917,7 +926,7 @@
       <c r="B9" s="9">
         <v>45534</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -938,7 +947,7 @@
       <c r="B10" s="9">
         <v>45534</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D10" s="11" t="s">
@@ -959,7 +968,7 @@
       <c r="B11" s="9">
         <v>45541</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="26">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D11" s="22" t="s">
@@ -978,7 +987,7 @@
       <c r="B12" s="9">
         <v>45541</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D12" s="22" t="s">
@@ -999,7 +1008,7 @@
       <c r="B13" s="9">
         <v>45541</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="26">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D13" s="22" t="s">
@@ -1018,7 +1027,7 @@
       <c r="B14" s="9">
         <v>45548</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="26">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D14" s="22" t="s">
@@ -1037,7 +1046,7 @@
       <c r="B15" s="9">
         <v>45548</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="26">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="D15" s="22" t="s">
@@ -1056,7 +1065,7 @@
       <c r="B16" s="9">
         <v>45548</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="26">
         <v>3.125E-2</v>
       </c>
       <c r="D16" s="22" t="s">
@@ -1075,7 +1084,7 @@
       <c r="B17" s="9">
         <v>45548</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="26">
         <v>2.4305555555555556E-2</v>
       </c>
       <c r="D17" s="22" t="s">
@@ -1096,7 +1105,7 @@
       <c r="B18" s="9">
         <v>45562</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="26">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="D18" s="11" t="s">
@@ -1115,7 +1124,7 @@
       <c r="B19" s="9">
         <v>45562</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="26">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D19" s="11" t="s">
@@ -1134,7 +1143,7 @@
       <c r="B20" s="9">
         <v>45562</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="26">
         <v>3.4722222222222224E-2</v>
       </c>
       <c r="D20" s="11" t="s">
@@ -1155,7 +1164,7 @@
       <c r="B21" s="9">
         <v>45562</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="26">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D21" s="11" t="s">
@@ -1174,7 +1183,7 @@
       <c r="B22" s="9">
         <v>45562</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="26">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -1195,7 +1204,7 @@
       <c r="B23" s="9">
         <v>45562</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="26">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D23" s="11" t="s">
@@ -1214,7 +1223,7 @@
       <c r="B24" s="9">
         <v>45562</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C24" s="26">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="D24" s="11" t="s">
@@ -1233,7 +1242,7 @@
       <c r="B25" s="9">
         <v>45563</v>
       </c>
-      <c r="C25" s="27">
+      <c r="C25" s="26">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="D25" s="11" t="s">
@@ -1254,7 +1263,7 @@
       <c r="B26" s="9">
         <v>45563</v>
       </c>
-      <c r="C26" s="27">
+      <c r="C26" s="26">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D26" s="11" t="s">
@@ -1275,7 +1284,7 @@
       <c r="B27" s="9">
         <v>45569</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="26">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D27" s="11" t="s">
@@ -1294,7 +1303,7 @@
       <c r="B28" s="9">
         <v>45569</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C28" s="26">
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="D28" s="11" t="s">
@@ -1315,14 +1324,14 @@
       <c r="B29" s="9">
         <v>45569</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C29" s="26">
         <v>9.7222222222222224E-2</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F29" s="11"/>
     </row>
@@ -1334,14 +1343,14 @@
       <c r="B30" s="9">
         <v>45569</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C30" s="26">
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F30" s="11"/>
     </row>
@@ -1353,14 +1362,14 @@
       <c r="B31" s="9">
         <v>45576</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C31" s="26">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F31" s="11"/>
     </row>
@@ -1372,14 +1381,14 @@
       <c r="B32" s="9">
         <v>45576</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C32" s="26">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>41</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1391,14 +1400,14 @@
       <c r="B33" s="9">
         <v>45576</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C33" s="26">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="11"/>
     </row>
@@ -1410,14 +1419,14 @@
       <c r="B34" s="9">
         <v>45576</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C34" s="26">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F34" s="11"/>
     </row>
@@ -1429,14 +1438,14 @@
       <c r="B35" s="9">
         <v>45576</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C35" s="26">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F35" s="11"/>
     </row>
@@ -1448,14 +1457,14 @@
       <c r="B36" s="9">
         <v>45576</v>
       </c>
-      <c r="C36" s="27">
+      <c r="C36" s="26">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F36" s="11"/>
     </row>
@@ -1467,14 +1476,14 @@
       <c r="B37" s="9">
         <v>45588</v>
       </c>
-      <c r="C37" s="27">
+      <c r="C37" s="26">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F37" s="11"/>
     </row>
@@ -1486,14 +1495,14 @@
       <c r="B38" s="9">
         <v>45588</v>
       </c>
-      <c r="C38" s="27">
+      <c r="C38" s="26">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F38" s="11"/>
     </row>
@@ -1505,14 +1514,14 @@
       <c r="B39" s="9">
         <v>45588</v>
       </c>
-      <c r="C39" s="27">
+      <c r="C39" s="26">
         <v>6.9444444444444448E-2</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F39" s="11"/>
     </row>
@@ -1524,14 +1533,14 @@
       <c r="B40" s="9">
         <v>45588</v>
       </c>
-      <c r="C40" s="27">
+      <c r="C40" s="26">
         <v>6.25E-2</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F40" s="11"/>
     </row>
@@ -1543,14 +1552,14 @@
       <c r="B41" s="9">
         <v>45589</v>
       </c>
-      <c r="C41" s="27">
+      <c r="C41" s="26">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F41" s="11"/>
     </row>
@@ -1562,14 +1571,14 @@
       <c r="B42" s="9">
         <v>45589</v>
       </c>
-      <c r="C42" s="27">
+      <c r="C42" s="26">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F42" s="11"/>
     </row>
@@ -1581,14 +1590,14 @@
       <c r="B43" s="9">
         <v>45589</v>
       </c>
-      <c r="C43" s="27">
+      <c r="C43" s="26">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F43" s="11"/>
     </row>
@@ -1600,14 +1609,14 @@
       <c r="B44" s="9">
         <v>45589</v>
       </c>
-      <c r="C44" s="27">
+      <c r="C44" s="26">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F44" s="11"/>
     </row>
@@ -1619,37 +1628,55 @@
       <c r="B45" s="9">
         <v>45589</v>
       </c>
-      <c r="C45" s="27">
+      <c r="C45" s="26">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F45" s="11"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="14" t="str">
+    <row r="46" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="A46" s="14">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B46" s="9">
+        <v>45591</v>
+      </c>
+      <c r="C46" s="26">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="14" t="str">
+      <c r="A47" s="14">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B47" s="9">
+        <v>45591</v>
+      </c>
+      <c r="C47" s="26">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="F47" s="11"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1658,7 +1685,7 @@
         <v/>
       </c>
       <c r="B48" s="9"/>
-      <c r="C48" s="27"/>
+      <c r="C48" s="26"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
@@ -1669,7 +1696,7 @@
         <v/>
       </c>
       <c r="B49" s="9"/>
-      <c r="C49" s="27"/>
+      <c r="C49" s="26"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
@@ -1680,7 +1707,7 @@
         <v/>
       </c>
       <c r="B50" s="9"/>
-      <c r="C50" s="27"/>
+      <c r="C50" s="26"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
@@ -1691,7 +1718,7 @@
         <v/>
       </c>
       <c r="B51" s="9"/>
-      <c r="C51" s="27"/>
+      <c r="C51" s="26"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -1702,7 +1729,7 @@
         <v/>
       </c>
       <c r="B52" s="9"/>
-      <c r="C52" s="27"/>
+      <c r="C52" s="26"/>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
@@ -1713,7 +1740,7 @@
         <v/>
       </c>
       <c r="B53" s="9"/>
-      <c r="C53" s="27"/>
+      <c r="C53" s="26"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
@@ -1724,7 +1751,7 @@
         <v/>
       </c>
       <c r="B54" s="9"/>
-      <c r="C54" s="27"/>
+      <c r="C54" s="26"/>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
@@ -1735,7 +1762,7 @@
         <v/>
       </c>
       <c r="B55" s="9"/>
-      <c r="C55" s="27"/>
+      <c r="C55" s="26"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -1746,7 +1773,7 @@
         <v/>
       </c>
       <c r="B56" s="9"/>
-      <c r="C56" s="27"/>
+      <c r="C56" s="26"/>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
@@ -1757,7 +1784,7 @@
         <v/>
       </c>
       <c r="B57" s="9"/>
-      <c r="C57" s="27"/>
+      <c r="C57" s="26"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
@@ -1768,7 +1795,7 @@
         <v/>
       </c>
       <c r="B58" s="9"/>
-      <c r="C58" s="27"/>
+      <c r="C58" s="26"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
@@ -1779,7 +1806,7 @@
         <v/>
       </c>
       <c r="B59" s="9"/>
-      <c r="C59" s="27"/>
+      <c r="C59" s="26"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
@@ -1790,7 +1817,7 @@
         <v/>
       </c>
       <c r="B60" s="9"/>
-      <c r="C60" s="27"/>
+      <c r="C60" s="26"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -1801,7 +1828,7 @@
         <v/>
       </c>
       <c r="B61" s="9"/>
-      <c r="C61" s="27"/>
+      <c r="C61" s="26"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
@@ -1812,7 +1839,7 @@
         <v/>
       </c>
       <c r="B62" s="9"/>
-      <c r="C62" s="27"/>
+      <c r="C62" s="26"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -1823,7 +1850,7 @@
         <v/>
       </c>
       <c r="B63" s="9"/>
-      <c r="C63" s="27"/>
+      <c r="C63" s="26"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
@@ -1834,7 +1861,7 @@
         <v/>
       </c>
       <c r="B64" s="9"/>
-      <c r="C64" s="27"/>
+      <c r="C64" s="26"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
@@ -1845,7 +1872,7 @@
         <v/>
       </c>
       <c r="B65" s="9"/>
-      <c r="C65" s="27"/>
+      <c r="C65" s="26"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
@@ -1856,7 +1883,7 @@
         <v/>
       </c>
       <c r="B66" s="9"/>
-      <c r="C66" s="27"/>
+      <c r="C66" s="26"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
@@ -1867,7 +1894,7 @@
         <v/>
       </c>
       <c r="B67" s="9"/>
-      <c r="C67" s="27"/>
+      <c r="C67" s="26"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
@@ -1878,7 +1905,7 @@
         <v/>
       </c>
       <c r="B68" s="9"/>
-      <c r="C68" s="27"/>
+      <c r="C68" s="26"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
@@ -1889,7 +1916,7 @@
         <v/>
       </c>
       <c r="B69" s="9"/>
-      <c r="C69" s="27"/>
+      <c r="C69" s="26"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
@@ -1900,7 +1927,7 @@
         <v/>
       </c>
       <c r="B70" s="9"/>
-      <c r="C70" s="27"/>
+      <c r="C70" s="26"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -1911,7 +1938,7 @@
         <v/>
       </c>
       <c r="B71" s="9"/>
-      <c r="C71" s="27"/>
+      <c r="C71" s="26"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
@@ -1922,7 +1949,7 @@
         <v/>
       </c>
       <c r="B72" s="9"/>
-      <c r="C72" s="27"/>
+      <c r="C72" s="26"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
@@ -1933,7 +1960,7 @@
         <v/>
       </c>
       <c r="B73" s="9"/>
-      <c r="C73" s="27"/>
+      <c r="C73" s="26"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
@@ -1944,7 +1971,7 @@
         <v/>
       </c>
       <c r="B74" s="9"/>
-      <c r="C74" s="27"/>
+      <c r="C74" s="26"/>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
@@ -1955,7 +1982,7 @@
         <v/>
       </c>
       <c r="B75" s="9"/>
-      <c r="C75" s="27"/>
+      <c r="C75" s="26"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
       <c r="F75" s="11"/>
@@ -1966,7 +1993,7 @@
         <v/>
       </c>
       <c r="B76" s="9"/>
-      <c r="C76" s="27"/>
+      <c r="C76" s="26"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
@@ -1977,7 +2004,7 @@
         <v/>
       </c>
       <c r="B77" s="9"/>
-      <c r="C77" s="27"/>
+      <c r="C77" s="26"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
@@ -1988,7 +2015,7 @@
         <v/>
       </c>
       <c r="B78" s="9"/>
-      <c r="C78" s="27"/>
+      <c r="C78" s="26"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
@@ -1999,7 +2026,7 @@
         <v/>
       </c>
       <c r="B79" s="9"/>
-      <c r="C79" s="27"/>
+      <c r="C79" s="26"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
@@ -2010,7 +2037,7 @@
         <v/>
       </c>
       <c r="B80" s="9"/>
-      <c r="C80" s="27"/>
+      <c r="C80" s="26"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
       <c r="F80" s="11"/>
@@ -2021,7 +2048,7 @@
         <v/>
       </c>
       <c r="B81" s="9"/>
-      <c r="C81" s="27"/>
+      <c r="C81" s="26"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
@@ -2032,7 +2059,7 @@
         <v/>
       </c>
       <c r="B82" s="9"/>
-      <c r="C82" s="27"/>
+      <c r="C82" s="26"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
       <c r="F82" s="11"/>
@@ -2043,7 +2070,7 @@
         <v/>
       </c>
       <c r="B83" s="9"/>
-      <c r="C83" s="27"/>
+      <c r="C83" s="26"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
@@ -2054,7 +2081,7 @@
         <v/>
       </c>
       <c r="B84" s="9"/>
-      <c r="C84" s="27"/>
+      <c r="C84" s="26"/>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
       <c r="F84" s="11"/>
@@ -2065,7 +2092,7 @@
         <v/>
       </c>
       <c r="B85" s="9"/>
-      <c r="C85" s="27"/>
+      <c r="C85" s="26"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
       <c r="F85" s="11"/>
@@ -2076,7 +2103,7 @@
         <v/>
       </c>
       <c r="B86" s="9"/>
-      <c r="C86" s="27"/>
+      <c r="C86" s="26"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
@@ -2087,7 +2114,7 @@
         <v/>
       </c>
       <c r="B87" s="9"/>
-      <c r="C87" s="27"/>
+      <c r="C87" s="26"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
@@ -2098,7 +2125,7 @@
         <v/>
       </c>
       <c r="B88" s="9"/>
-      <c r="C88" s="27"/>
+      <c r="C88" s="26"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
@@ -2109,7 +2136,7 @@
         <v/>
       </c>
       <c r="B89" s="9"/>
-      <c r="C89" s="27"/>
+      <c r="C89" s="26"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
@@ -2120,7 +2147,7 @@
         <v/>
       </c>
       <c r="B90" s="9"/>
-      <c r="C90" s="27"/>
+      <c r="C90" s="26"/>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
@@ -2131,7 +2158,7 @@
         <v/>
       </c>
       <c r="B91" s="9"/>
-      <c r="C91" s="27"/>
+      <c r="C91" s="26"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
@@ -2142,7 +2169,7 @@
         <v/>
       </c>
       <c r="B92" s="9"/>
-      <c r="C92" s="27"/>
+      <c r="C92" s="26"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
       <c r="F92" s="11"/>
@@ -2153,7 +2180,7 @@
         <v/>
       </c>
       <c r="B93" s="9"/>
-      <c r="C93" s="27"/>
+      <c r="C93" s="26"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
       <c r="F93" s="11"/>
@@ -2164,7 +2191,7 @@
         <v/>
       </c>
       <c r="B94" s="9"/>
-      <c r="C94" s="27"/>
+      <c r="C94" s="26"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
       <c r="F94" s="11"/>
@@ -2175,7 +2202,7 @@
         <v/>
       </c>
       <c r="B95" s="9"/>
-      <c r="C95" s="27"/>
+      <c r="C95" s="26"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
@@ -2186,7 +2213,7 @@
         <v/>
       </c>
       <c r="B96" s="9"/>
-      <c r="C96" s="27"/>
+      <c r="C96" s="26"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
@@ -2197,7 +2224,7 @@
         <v/>
       </c>
       <c r="B97" s="9"/>
-      <c r="C97" s="27"/>
+      <c r="C97" s="26"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
@@ -2208,7 +2235,7 @@
         <v/>
       </c>
       <c r="B98" s="9"/>
-      <c r="C98" s="27"/>
+      <c r="C98" s="26"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
@@ -2219,7 +2246,7 @@
         <v/>
       </c>
       <c r="B99" s="9"/>
-      <c r="C99" s="27"/>
+      <c r="C99" s="26"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
@@ -2230,7 +2257,7 @@
         <v/>
       </c>
       <c r="B100" s="9"/>
-      <c r="C100" s="27"/>
+      <c r="C100" s="26"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
@@ -2241,7 +2268,7 @@
         <v/>
       </c>
       <c r="B101" s="9"/>
-      <c r="C101" s="27"/>
+      <c r="C101" s="26"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
       <c r="F101" s="11"/>
@@ -2252,7 +2279,7 @@
         <v/>
       </c>
       <c r="B102" s="9"/>
-      <c r="C102" s="27"/>
+      <c r="C102" s="26"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
@@ -2263,7 +2290,7 @@
         <v/>
       </c>
       <c r="B103" s="9"/>
-      <c r="C103" s="27"/>
+      <c r="C103" s="26"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
       <c r="F103" s="11"/>
@@ -2274,7 +2301,7 @@
         <v/>
       </c>
       <c r="B104" s="9"/>
-      <c r="C104" s="27"/>
+      <c r="C104" s="26"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
@@ -2285,7 +2312,7 @@
         <v/>
       </c>
       <c r="B105" s="9"/>
-      <c r="C105" s="27"/>
+      <c r="C105" s="26"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
       <c r="F105" s="11"/>
@@ -2296,7 +2323,7 @@
         <v/>
       </c>
       <c r="B106" s="9"/>
-      <c r="C106" s="27"/>
+      <c r="C106" s="26"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
       <c r="F106" s="11"/>
@@ -2307,7 +2334,7 @@
         <v/>
       </c>
       <c r="B107" s="9"/>
-      <c r="C107" s="27"/>
+      <c r="C107" s="26"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
       <c r="F107" s="11"/>
@@ -2318,7 +2345,7 @@
         <v/>
       </c>
       <c r="B108" s="9"/>
-      <c r="C108" s="27"/>
+      <c r="C108" s="26"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
@@ -2329,7 +2356,7 @@
         <v/>
       </c>
       <c r="B109" s="9"/>
-      <c r="C109" s="27"/>
+      <c r="C109" s="26"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
       <c r="F109" s="11"/>
@@ -2340,7 +2367,7 @@
         <v/>
       </c>
       <c r="B110" s="9"/>
-      <c r="C110" s="27"/>
+      <c r="C110" s="26"/>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
       <c r="F110" s="11"/>
@@ -2351,7 +2378,7 @@
         <v/>
       </c>
       <c r="B111" s="9"/>
-      <c r="C111" s="27"/>
+      <c r="C111" s="26"/>
       <c r="D111" s="11"/>
       <c r="E111" s="11"/>
       <c r="F111" s="11"/>
@@ -2362,7 +2389,7 @@
         <v/>
       </c>
       <c r="B112" s="9"/>
-      <c r="C112" s="27"/>
+      <c r="C112" s="26"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
       <c r="F112" s="11"/>
@@ -2373,7 +2400,7 @@
         <v/>
       </c>
       <c r="B113" s="9"/>
-      <c r="C113" s="27"/>
+      <c r="C113" s="26"/>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
       <c r="F113" s="11"/>
@@ -2384,7 +2411,7 @@
         <v/>
       </c>
       <c r="B114" s="9"/>
-      <c r="C114" s="27"/>
+      <c r="C114" s="26"/>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
       <c r="F114" s="11"/>
@@ -2395,7 +2422,7 @@
         <v/>
       </c>
       <c r="B115" s="9"/>
-      <c r="C115" s="27"/>
+      <c r="C115" s="26"/>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
       <c r="F115" s="11"/>
@@ -2406,7 +2433,7 @@
         <v/>
       </c>
       <c r="B116" s="9"/>
-      <c r="C116" s="27"/>
+      <c r="C116" s="26"/>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
@@ -2417,7 +2444,7 @@
         <v/>
       </c>
       <c r="B117" s="9"/>
-      <c r="C117" s="27"/>
+      <c r="C117" s="26"/>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
       <c r="F117" s="11"/>
@@ -2428,7 +2455,7 @@
         <v/>
       </c>
       <c r="B118" s="9"/>
-      <c r="C118" s="27"/>
+      <c r="C118" s="26"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
@@ -2439,7 +2466,7 @@
         <v/>
       </c>
       <c r="B119" s="9"/>
-      <c r="C119" s="27"/>
+      <c r="C119" s="26"/>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
       <c r="F119" s="11"/>
@@ -2450,7 +2477,7 @@
         <v/>
       </c>
       <c r="B120" s="9"/>
-      <c r="C120" s="27"/>
+      <c r="C120" s="26"/>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
       <c r="F120" s="11"/>
@@ -2461,7 +2488,7 @@
         <v/>
       </c>
       <c r="B121" s="9"/>
-      <c r="C121" s="27"/>
+      <c r="C121" s="26"/>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
       <c r="F121" s="11"/>
@@ -2472,7 +2499,7 @@
         <v/>
       </c>
       <c r="B122" s="9"/>
-      <c r="C122" s="27"/>
+      <c r="C122" s="26"/>
       <c r="D122" s="11"/>
       <c r="E122" s="11"/>
       <c r="F122" s="11"/>
@@ -2483,7 +2510,7 @@
         <v/>
       </c>
       <c r="B123" s="9"/>
-      <c r="C123" s="27"/>
+      <c r="C123" s="26"/>
       <c r="D123" s="11"/>
       <c r="E123" s="11"/>
       <c r="F123" s="11"/>
@@ -2494,7 +2521,7 @@
         <v/>
       </c>
       <c r="B124" s="9"/>
-      <c r="C124" s="27"/>
+      <c r="C124" s="26"/>
       <c r="D124" s="11"/>
       <c r="E124" s="11"/>
       <c r="F124" s="11"/>
@@ -2505,7 +2532,7 @@
         <v/>
       </c>
       <c r="B125" s="9"/>
-      <c r="C125" s="27"/>
+      <c r="C125" s="26"/>
       <c r="D125" s="11"/>
       <c r="E125" s="11"/>
       <c r="F125" s="11"/>
@@ -2516,7 +2543,7 @@
         <v/>
       </c>
       <c r="B126" s="9"/>
-      <c r="C126" s="27"/>
+      <c r="C126" s="26"/>
       <c r="D126" s="11"/>
       <c r="E126" s="11"/>
       <c r="F126" s="11"/>
@@ -2527,7 +2554,7 @@
         <v/>
       </c>
       <c r="B127" s="9"/>
-      <c r="C127" s="27"/>
+      <c r="C127" s="26"/>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
       <c r="F127" s="11"/>
@@ -2538,7 +2565,7 @@
         <v/>
       </c>
       <c r="B128" s="9"/>
-      <c r="C128" s="27"/>
+      <c r="C128" s="26"/>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
       <c r="F128" s="11"/>
@@ -2549,7 +2576,7 @@
         <v/>
       </c>
       <c r="B129" s="9"/>
-      <c r="C129" s="27"/>
+      <c r="C129" s="26"/>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
       <c r="F129" s="11"/>
@@ -2560,7 +2587,7 @@
         <v/>
       </c>
       <c r="B130" s="9"/>
-      <c r="C130" s="27"/>
+      <c r="C130" s="26"/>
       <c r="D130" s="11"/>
       <c r="E130" s="11"/>
       <c r="F130" s="11"/>
@@ -2571,7 +2598,7 @@
         <v/>
       </c>
       <c r="B131" s="9"/>
-      <c r="C131" s="27"/>
+      <c r="C131" s="26"/>
       <c r="D131" s="11"/>
       <c r="E131" s="11"/>
       <c r="F131" s="11"/>
@@ -2582,7 +2609,7 @@
         <v/>
       </c>
       <c r="B132" s="9"/>
-      <c r="C132" s="27"/>
+      <c r="C132" s="26"/>
       <c r="D132" s="11"/>
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
@@ -2593,7 +2620,7 @@
         <v/>
       </c>
       <c r="B133" s="9"/>
-      <c r="C133" s="27"/>
+      <c r="C133" s="26"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11"/>
       <c r="F133" s="11"/>
@@ -2604,7 +2631,7 @@
         <v/>
       </c>
       <c r="B134" s="9"/>
-      <c r="C134" s="27"/>
+      <c r="C134" s="26"/>
       <c r="D134" s="11"/>
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
@@ -2615,7 +2642,7 @@
         <v/>
       </c>
       <c r="B135" s="9"/>
-      <c r="C135" s="27"/>
+      <c r="C135" s="26"/>
       <c r="D135" s="11"/>
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
@@ -2626,7 +2653,7 @@
         <v/>
       </c>
       <c r="B136" s="9"/>
-      <c r="C136" s="27"/>
+      <c r="C136" s="26"/>
       <c r="D136" s="11"/>
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
@@ -2637,7 +2664,7 @@
         <v/>
       </c>
       <c r="B137" s="9"/>
-      <c r="C137" s="27"/>
+      <c r="C137" s="26"/>
       <c r="D137" s="11"/>
       <c r="E137" s="11"/>
       <c r="F137" s="11"/>
@@ -2648,7 +2675,7 @@
         <v/>
       </c>
       <c r="B138" s="9"/>
-      <c r="C138" s="27"/>
+      <c r="C138" s="26"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
       <c r="F138" s="11"/>
@@ -2659,7 +2686,7 @@
         <v/>
       </c>
       <c r="B139" s="9"/>
-      <c r="C139" s="27"/>
+      <c r="C139" s="26"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
       <c r="F139" s="11"/>
@@ -2670,7 +2697,7 @@
         <v/>
       </c>
       <c r="B140" s="9"/>
-      <c r="C140" s="27"/>
+      <c r="C140" s="26"/>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
       <c r="F140" s="11"/>
@@ -2681,7 +2708,7 @@
         <v/>
       </c>
       <c r="B141" s="9"/>
-      <c r="C141" s="27"/>
+      <c r="C141" s="26"/>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
       <c r="F141" s="11"/>
@@ -2692,7 +2719,7 @@
         <v/>
       </c>
       <c r="B142" s="9"/>
-      <c r="C142" s="27"/>
+      <c r="C142" s="26"/>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
       <c r="F142" s="11"/>
@@ -2703,7 +2730,7 @@
         <v/>
       </c>
       <c r="B143" s="9"/>
-      <c r="C143" s="27"/>
+      <c r="C143" s="26"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
       <c r="F143" s="11"/>
@@ -2714,7 +2741,7 @@
         <v/>
       </c>
       <c r="B144" s="9"/>
-      <c r="C144" s="27"/>
+      <c r="C144" s="26"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
       <c r="F144" s="11"/>
@@ -2725,7 +2752,7 @@
         <v/>
       </c>
       <c r="B145" s="9"/>
-      <c r="C145" s="27"/>
+      <c r="C145" s="26"/>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
       <c r="F145" s="11"/>
@@ -2736,7 +2763,7 @@
         <v/>
       </c>
       <c r="B146" s="9"/>
-      <c r="C146" s="27"/>
+      <c r="C146" s="26"/>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
       <c r="F146" s="11"/>
@@ -7038,15 +7065,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7269,6 +7287,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
   <ds:schemaRefs>
@@ -7281,14 +7308,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7305,4 +7324,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(documentaion): add the IA part of the documentation
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyco\Documents\GitHub\plot-that-lines\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5208CC5-861B-40E4-9EBA-27BB43C301DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89F0A5E-B98B-4311-AE3B-856540F317AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -257,6 +257,18 @@
   </si>
   <si>
     <t>J'avance dans le rapport à fournir. Il ne reste plue que le IceScrub.</t>
+  </si>
+  <si>
+    <t>Je gère les erreurs potentiels puis je rajoute la fonctionnalité de trier les données grâce à la méthode anciennement créé.</t>
+  </si>
+  <si>
+    <t>Je réduis mon nombre d'appel à l'API</t>
+  </si>
+  <si>
+    <t>Rajouter les légendes au graphique</t>
+  </si>
+  <si>
+    <t>Je mets mon rapport à jour par rapport à ce que j'ai rajouté. Puis je rajoute les IceTools.</t>
   </si>
 </sst>
 </file>
@@ -753,9 +765,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -823,7 +835,7 @@
       </c>
       <c r="C3" s="27">
         <f>SUM(C6:C521)</f>
-        <v>1.2152777777777775</v>
+        <v>1.3611111111111107</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1679,48 +1691,80 @@
       </c>
       <c r="F47" s="11"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="14" t="str">
+    <row r="48" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="A48" s="14">
         <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="B48" s="9">
+        <v>45595</v>
+      </c>
+      <c r="C48" s="26">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="14" t="str">
+      <c r="A49" s="14">
         <f>IF(ISBLANK(B49),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="B49" s="9">
+        <v>45595</v>
+      </c>
+      <c r="C49" s="26">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="F49" s="11"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="14" t="str">
+      <c r="A50" s="14">
         <f>IF(ISBLANK(B50),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="B50" s="9">
+        <v>45595</v>
+      </c>
+      <c r="C50" s="26">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>74</v>
+      </c>
       <c r="F50" s="11"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="14" t="str">
+      <c r="A51" s="14">
         <f>IF(ISBLANK(B51),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="B51" s="9">
+        <v>45595</v>
+      </c>
+      <c r="C51" s="26">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>75</v>
+      </c>
       <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -7065,6 +7109,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7287,15 +7340,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
   <ds:schemaRefs>
@@ -7308,6 +7352,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7324,12 +7376,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>